<commit_message>
OpenDMX Test (funktionierte leider nicht, DLL in Verwendung (geht nicht am Mac)), UDP Test (senden und empfangen funktioniert), Erste versuche DMX Protokoll (geht nicht), ESP Konfiguration ausgelesen, Zeitblätter
</commit_message>
<xml_diff>
--- a/Zeitblätter/Ursus Schneider.xlsx
+++ b/Zeitblätter/Ursus Schneider.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oktober" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>Datum</t>
   </si>
@@ -102,6 +102,18 @@
   </si>
   <si>
     <t>14:00 - 14:30</t>
+  </si>
+  <si>
+    <t>14:00 - 15:30, 19:00 - 21:30</t>
+  </si>
+  <si>
+    <t>DMX Tests in FH, OpenDMX test, UDP funktioniert</t>
+  </si>
+  <si>
+    <t>Dokumentation</t>
+  </si>
+  <si>
+    <t>08:00 - 08:30</t>
   </si>
 </sst>
 </file>
@@ -447,7 +459,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -659,11 +671,29 @@
         <f t="shared" si="0"/>
         <v>42660</v>
       </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>42661</v>
+      </c>
+      <c r="B21">
+        <v>0.5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -753,7 +783,7 @@
       </c>
       <c r="B36" s="2">
         <f>SUM(B5:B34)</f>
-        <v>22</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>